<commit_message>
added whole new strategy based on unemployment rate, added its corresponding methods to the new class. working on abstraction and reutilization of code
</commit_message>
<xml_diff>
--- a/backtesting/excelStats/general_stats.xlsx
+++ b/backtesting/excelStats/general_stats.xlsx
@@ -594,58 +594,58 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.33</v>
+        <v>0.05</v>
       </c>
       <c r="C4" t="n">
-        <v>0.26</v>
+        <v>0.03</v>
       </c>
       <c r="D4" t="n">
-        <v>0.32</v>
+        <v>0.04</v>
       </c>
       <c r="E4" t="n">
-        <v>3.42</v>
+        <v>0.99</v>
       </c>
       <c r="F4" t="n">
-        <v>24.37</v>
+        <v>11.58</v>
       </c>
       <c r="G4" t="n">
-        <v>-18.45</v>
+        <v>-20.47</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
       </c>
       <c r="I4" t="n">
-        <v>0.1</v>
+        <v>0.03</v>
       </c>
       <c r="J4" t="n">
-        <v>0.15</v>
+        <v>0.04</v>
       </c>
       <c r="K4" t="n">
-        <v>3.28</v>
+        <v>0.8</v>
       </c>
       <c r="L4" t="n">
-        <v>24.37</v>
+        <v>9.1</v>
       </c>
       <c r="M4" t="n">
-        <v>-17.16</v>
+        <v>-20.47</v>
       </c>
       <c r="N4" t="n">
-        <v>0.08</v>
+        <v>0.05</v>
       </c>
       <c r="O4" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="P4" t="n">
         <v>0.04</v>
       </c>
-      <c r="P4" t="n">
-        <v>0.05</v>
-      </c>
       <c r="Q4" t="n">
-        <v>1.42</v>
+        <v>0.99</v>
       </c>
       <c r="R4" t="n">
-        <v>9.380000000000001</v>
+        <v>11.58</v>
       </c>
       <c r="S4" t="n">
-        <v>-11.98</v>
+        <v>-20.47</v>
       </c>
     </row>
     <row r="5">
@@ -655,58 +655,58 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
       <c r="C5" t="n">
-        <v>0.33</v>
+        <v>0.04</v>
       </c>
       <c r="D5" t="n">
-        <v>0.37</v>
+        <v>0.04</v>
       </c>
       <c r="E5" t="n">
-        <v>3</v>
+        <v>0.87</v>
       </c>
       <c r="F5" t="n">
-        <v>24.37</v>
+        <v>9.1</v>
       </c>
       <c r="G5" t="n">
-        <v>-9.279999999999999</v>
+        <v>-20.47</v>
       </c>
       <c r="H5" t="n">
-        <v>0.26</v>
+        <v>0.06</v>
       </c>
       <c r="I5" t="n">
-        <v>0.33</v>
+        <v>0.04</v>
       </c>
       <c r="J5" t="n">
-        <v>0.37</v>
+        <v>0.04</v>
       </c>
       <c r="K5" t="n">
-        <v>3</v>
+        <v>0.87</v>
       </c>
       <c r="L5" t="n">
-        <v>24.37</v>
+        <v>9.1</v>
       </c>
       <c r="M5" t="n">
-        <v>-9.279999999999999</v>
+        <v>-20.47</v>
       </c>
       <c r="N5" t="n">
-        <v>0.12</v>
+        <v>0.06</v>
       </c>
       <c r="O5" t="n">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="P5" t="n">
-        <v>0.09</v>
+        <v>0.04</v>
       </c>
       <c r="Q5" t="n">
-        <v>1.11</v>
+        <v>0.87</v>
       </c>
       <c r="R5" t="n">
-        <v>7.03</v>
+        <v>9.1</v>
       </c>
       <c r="S5" t="n">
-        <v>-5.89</v>
+        <v>-20.47</v>
       </c>
     </row>
     <row r="6">
@@ -716,22 +716,22 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.41</v>
+        <v>-0.01</v>
       </c>
       <c r="C6" t="n">
-        <v>0.41</v>
+        <v>-0.02</v>
       </c>
       <c r="D6" t="n">
-        <v>0.48</v>
+        <v>-0.01</v>
       </c>
       <c r="E6" t="n">
-        <v>3.79</v>
+        <v>1.49</v>
       </c>
       <c r="F6" t="n">
-        <v>14.33</v>
+        <v>11.58</v>
       </c>
       <c r="G6" t="n">
-        <v>-8.029999999999999</v>
+        <v>-11.98</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -752,22 +752,22 @@
         <v>0</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.1</v>
+        <v>-0.01</v>
       </c>
       <c r="O6" t="n">
-        <v>0.08</v>
+        <v>-0.02</v>
       </c>
       <c r="P6" t="n">
-        <v>0.09</v>
+        <v>-0.01</v>
       </c>
       <c r="Q6" t="n">
-        <v>1.44</v>
+        <v>1.49</v>
       </c>
       <c r="R6" t="n">
-        <v>5.54</v>
+        <v>11.58</v>
       </c>
       <c r="S6" t="n">
-        <v>-2.91</v>
+        <v>-11.98</v>
       </c>
     </row>
     <row r="7">
@@ -776,60 +776,24 @@
           <t>vendido</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="E7" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="F7" t="n">
-        <v>17.16</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-18.45</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-0.44</v>
-      </c>
-      <c r="I7" t="n">
-        <v>-0.27</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-0.19</v>
-      </c>
-      <c r="K7" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="L7" t="n">
-        <v>18.45</v>
-      </c>
-      <c r="M7" t="n">
-        <v>-17.16</v>
-      </c>
-      <c r="N7" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="O7" t="n">
-        <v>-0.03</v>
-      </c>
-      <c r="P7" t="n">
-        <v>-0.02</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>1.83</v>
-      </c>
-      <c r="R7" t="n">
-        <v>9.380000000000001</v>
-      </c>
-      <c r="S7" t="n">
-        <v>-11.98</v>
-      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
+      <c r="Q7" t="inlineStr"/>
+      <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>